<commit_message>
added generate ppmp file function
</commit_message>
<xml_diff>
--- a/storage/app/public/templates/ppmp_template.xlsx
+++ b/storage/app/public/templates/ppmp_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo-User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A78EAE-F989-4A9D-AD20-78909F46149C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB24D847-730C-4773-B90F-F025199F9C07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{D041A653-07EE-4EC8-A9FC-654FA94700C5}"/>
   </bookViews>
@@ -185,7 +185,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,14 +219,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -282,7 +274,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -368,51 +360,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -423,9 +509,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -441,39 +524,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -854,8 +905,8 @@
   </sheetPr>
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:F24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,270 +921,270 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
     </row>
     <row r="2" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="33" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="30" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="30" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="30" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="17" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="17" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="18" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
     </row>
     <row r="8" spans="1:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-    </row>
-    <row r="12" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="39"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="20"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1171,204 +1222,204 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="5"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-    </row>
-    <row r="16" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="5"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="5"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-    </row>
-    <row r="18" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-    </row>
-    <row r="22" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="22">
+      <c r="B22" s="40"/>
+      <c r="C22" s="39">
         <f>SUM(F14:F20)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="22">
+      <c r="B23" s="41"/>
+      <c r="C23" s="39">
         <f>C22*0.1</f>
         <v>0</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="22">
+      <c r="B24" s="41"/>
+      <c r="C24" s="39">
         <f>C22*0.1</f>
         <v>0</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="22">
+      <c r="B25" s="42"/>
+      <c r="C25" s="39">
         <f>SUM(C22:F24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1386,62 +1437,95 @@
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="M30" s="13" t="s">
+      <c r="B30" s="8"/>
+      <c r="M30" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="13"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="13"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="9"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C32:S32"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="A2:B5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:L7"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="C33:S33"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:S12"/>
@@ -1458,39 +1542,6 @@
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="B12:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A2:B5"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:L7"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C32:S32"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
added ppmp form template serial numbers
</commit_message>
<xml_diff>
--- a/storage/app/public/templates/ppmp_template.xlsx
+++ b/storage/app/public/templates/ppmp_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo-User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB24D847-730C-4773-B90F-F025199F9C07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05E98E7-13BE-4A92-A9F9-61568BA44EAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{D041A653-07EE-4EC8-A9FC-654FA94700C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>TECHNOLOGICAL UNIVERSITY OF THE PHILIPPINES</t>
   </si>
@@ -175,6 +175,21 @@
   </si>
   <si>
     <t>Projects, Programs and Activity (PAPs)</t>
+  </si>
+  <si>
+    <t>F-BUD-8.3-PMP</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>07042018</t>
+  </si>
+  <si>
+    <t>1 / 1</t>
+  </si>
+  <si>
+    <t>CC-07042018</t>
   </si>
 </sst>
 </file>
@@ -409,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -443,62 +458,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -509,6 +471,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -524,8 +489,61 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -905,8 +923,8 @@
   </sheetPr>
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:J9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,16 +939,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
     </row>
     <row r="2" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="32" t="s">
         <v>0</v>
       </c>
@@ -943,90 +961,98 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="34" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="34" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="35" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
@@ -1045,15 +1071,17 @@
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
@@ -1068,15 +1096,17 @@
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
-      <c r="M7" s="36" t="s">
+      <c r="M7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
     </row>
     <row r="8" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1104,13 +1134,13 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="6"/>
@@ -1126,13 +1156,13 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
@@ -1143,48 +1173,48 @@
       <c r="R10" s="7"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="40"/>
+      <c r="D12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="20"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="37"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1224,10 +1254,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="44"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="13"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -1245,8 +1275,8 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="14"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
@@ -1266,8 +1296,8 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="14"/>
       <c r="E16" s="12"/>
       <c r="F16" s="13"/>
@@ -1287,8 +1317,8 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="14"/>
       <c r="E17" s="12"/>
       <c r="F17" s="13"/>
@@ -1308,8 +1338,8 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="14"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
@@ -1329,8 +1359,8 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="14"/>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
@@ -1350,8 +1380,8 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="14"/>
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
@@ -1370,56 +1400,56 @@
       <c r="S20" s="14"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="39">
+      <c r="B22" s="22"/>
+      <c r="C22" s="21">
         <f>SUM(F14:F20)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="39">
+      <c r="B23" s="23"/>
+      <c r="C23" s="21">
         <f>C22*0.1</f>
         <v>0</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="39">
+      <c r="B24" s="23"/>
+      <c r="C24" s="21">
         <f>C22*0.1</f>
         <v>0</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="39">
+      <c r="B25" s="24"/>
+      <c r="C25" s="21">
         <f>SUM(C22:F24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1446,53 +1476,86 @@
       <c r="P30" s="9"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:S12"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A2:B5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:L7"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="P1:R1"/>
@@ -1509,39 +1572,6 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="A2:B5"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:L7"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:S12"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>